<commit_message>
New results - H2 case study
</commit_message>
<xml_diff>
--- a/hypatia/results_planning/aggregation_config_planning.xlsx
+++ b/hypatia/results_planning/aggregation_config_planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SESAM\anaconda3\envs\hypatia\Lib\site-packages\hypatia\results_planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10530003_polimi_it/Documents/Desktop/hypatia/results_planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0D155F-8AB3-4055-BFFC-2D6E7A16B464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{1D0D155F-8AB3-4055-BFFC-2D6E7A16B464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{23349F99-3CDF-414C-BA75-E185E90516C4}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Techs" sheetId="1" r:id="rId1"/>
@@ -5301,7 +5301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -5319,9 +5319,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -30180,10 +30177,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC6584BC-59EB-4718-8D34-F6C00E857BCB}">
-  <dimension ref="A1:B75"/>
+  <dimension ref="A1:B74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A77" sqref="A75:B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -30783,9 +30780,6 @@
       <c r="B74" s="3" t="s">
         <v>1727</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A75" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>